<commit_message>
update dari laptop arif
</commit_message>
<xml_diff>
--- a/hasil_prediksi.xlsx
+++ b/hasil_prediksi.xlsx
@@ -453,7 +453,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Awas</t>
+          <t>Waspada</t>
         </is>
       </c>
     </row>
@@ -489,7 +489,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Aman</t>
+          <t>Waspada</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Aman</t>
+          <t>Waspada</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Siaga</t>
+          <t>Waspada</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Waspada</t>
+          <t>Aman</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Aman</t>
+          <t>Waspada</t>
         </is>
       </c>
     </row>
@@ -597,7 +597,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Awas</t>
+          <t>Waspada</t>
         </is>
       </c>
     </row>
@@ -609,7 +609,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Aman</t>
+          <t>Waspada</t>
         </is>
       </c>
     </row>
@@ -633,7 +633,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Siaga</t>
+          <t>Waspada</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Siaga</t>
+          <t>Waspada</t>
         </is>
       </c>
     </row>

</xml_diff>